<commit_message>
02.02.2021 MC Sales Detials
</commit_message>
<xml_diff>
--- a/2021/February/01.02.2021/MC Bank Statement Feb-2021.xlsx
+++ b/2021/February/01.02.2021/MC Bank Statement Feb-2021.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Feb 2021" sheetId="7" r:id="rId1"/>
     <sheet name="Expence" sheetId="15" r:id="rId2"/>
     <sheet name="Balance Transfer" sheetId="14" r:id="rId3"/>
     <sheet name="CAPITAL" sheetId="10" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="209">
   <si>
     <t>Date</t>
   </si>
@@ -1915,7 +1917,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="329">
+  <cellXfs count="331">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2728,6 +2730,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2755,12 +2775,6 @@
     <xf numFmtId="1" fontId="39" fillId="35" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2773,18 +2787,6 @@
     <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="39" fillId="35" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2856,6 +2858,12 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="21" fontId="39" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -2948,7 +2956,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2960,7 +2968,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2983,14 +2991,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3078,7 +3086,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3090,7 +3098,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3113,14 +3121,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3152,7 +3160,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3164,7 +3172,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3187,14 +3195,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4605,73 +4613,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="292" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
-      <c r="Q1" s="286"/>
-      <c r="R1" s="286"/>
-      <c r="S1" s="286"/>
+      <c r="B1" s="292"/>
+      <c r="C1" s="292"/>
+      <c r="D1" s="292"/>
+      <c r="E1" s="292"/>
+      <c r="F1" s="292"/>
+      <c r="G1" s="292"/>
+      <c r="H1" s="292"/>
+      <c r="I1" s="292"/>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+      <c r="L1" s="292"/>
+      <c r="M1" s="292"/>
+      <c r="N1" s="292"/>
+      <c r="O1" s="292"/>
+      <c r="P1" s="292"/>
+      <c r="Q1" s="292"/>
+      <c r="R1" s="292"/>
+      <c r="S1" s="292"/>
     </row>
     <row r="2" spans="1:26" s="198" customFormat="1" ht="18">
-      <c r="A2" s="287" t="s">
+      <c r="A2" s="293" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="287"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287"/>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="287"/>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
-      <c r="P2" s="287"/>
-      <c r="Q2" s="287"/>
-      <c r="R2" s="287"/>
-      <c r="S2" s="287"/>
+      <c r="B2" s="293"/>
+      <c r="C2" s="293"/>
+      <c r="D2" s="293"/>
+      <c r="E2" s="293"/>
+      <c r="F2" s="293"/>
+      <c r="G2" s="293"/>
+      <c r="H2" s="293"/>
+      <c r="I2" s="293"/>
+      <c r="J2" s="293"/>
+      <c r="K2" s="293"/>
+      <c r="L2" s="293"/>
+      <c r="M2" s="293"/>
+      <c r="N2" s="293"/>
+      <c r="O2" s="293"/>
+      <c r="P2" s="293"/>
+      <c r="Q2" s="293"/>
+      <c r="R2" s="293"/>
+      <c r="S2" s="293"/>
     </row>
     <row r="3" spans="1:26" s="199" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A3" s="288" t="s">
+      <c r="A3" s="294" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="289"/>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289"/>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
-      <c r="M3" s="289"/>
-      <c r="N3" s="289"/>
-      <c r="O3" s="289"/>
-      <c r="P3" s="289"/>
-      <c r="Q3" s="289"/>
-      <c r="R3" s="289"/>
-      <c r="S3" s="290"/>
+      <c r="B3" s="295"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="295"/>
+      <c r="E3" s="295"/>
+      <c r="F3" s="295"/>
+      <c r="G3" s="295"/>
+      <c r="H3" s="295"/>
+      <c r="I3" s="295"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="295"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="295"/>
+      <c r="N3" s="295"/>
+      <c r="O3" s="295"/>
+      <c r="P3" s="295"/>
+      <c r="Q3" s="295"/>
+      <c r="R3" s="295"/>
+      <c r="S3" s="296"/>
       <c r="U3" s="114"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
@@ -4680,58 +4688,58 @@
       <c r="Z3" s="29"/>
     </row>
     <row r="4" spans="1:26" s="201" customFormat="1">
-      <c r="A4" s="291" t="s">
+      <c r="A4" s="297" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="293" t="s">
+      <c r="B4" s="299" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="295" t="s">
+      <c r="C4" s="286" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="295" t="s">
+      <c r="D4" s="286" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="295" t="s">
+      <c r="E4" s="286" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="295" t="s">
+      <c r="F4" s="286" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="295" t="s">
+      <c r="G4" s="286" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="295" t="s">
+      <c r="H4" s="286" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="295" t="s">
+      <c r="I4" s="286" t="s">
         <v>125</v>
       </c>
-      <c r="J4" s="295" t="s">
+      <c r="J4" s="286" t="s">
         <v>104</v>
       </c>
-      <c r="K4" s="295" t="s">
+      <c r="K4" s="286" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="295" t="s">
+      <c r="L4" s="286" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="295" t="s">
+      <c r="M4" s="286" t="s">
         <v>107</v>
       </c>
-      <c r="N4" s="295" t="s">
+      <c r="N4" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="301" t="s">
+      <c r="O4" s="288" t="s">
         <v>170</v>
       </c>
-      <c r="P4" s="303" t="s">
+      <c r="P4" s="290" t="s">
         <v>109</v>
       </c>
-      <c r="Q4" s="299" t="s">
+      <c r="Q4" s="303" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="297" t="s">
+      <c r="R4" s="301" t="s">
         <v>110</v>
       </c>
       <c r="S4" s="200" t="s">
@@ -4744,24 +4752,24 @@
       <c r="Y4" s="203"/>
     </row>
     <row r="5" spans="1:26" s="201" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A5" s="292"/>
-      <c r="B5" s="294"/>
-      <c r="C5" s="296"/>
-      <c r="D5" s="296"/>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
-      <c r="G5" s="296"/>
-      <c r="H5" s="296"/>
-      <c r="I5" s="296"/>
-      <c r="J5" s="296"/>
-      <c r="K5" s="296"/>
-      <c r="L5" s="296"/>
-      <c r="M5" s="296"/>
-      <c r="N5" s="296"/>
-      <c r="O5" s="302"/>
-      <c r="P5" s="304"/>
-      <c r="Q5" s="300"/>
-      <c r="R5" s="298"/>
+      <c r="A5" s="298"/>
+      <c r="B5" s="300"/>
+      <c r="C5" s="287"/>
+      <c r="D5" s="287"/>
+      <c r="E5" s="287"/>
+      <c r="F5" s="287"/>
+      <c r="G5" s="287"/>
+      <c r="H5" s="287"/>
+      <c r="I5" s="287"/>
+      <c r="J5" s="287"/>
+      <c r="K5" s="287"/>
+      <c r="L5" s="287"/>
+      <c r="M5" s="287"/>
+      <c r="N5" s="287"/>
+      <c r="O5" s="289"/>
+      <c r="P5" s="291"/>
+      <c r="Q5" s="304"/>
+      <c r="R5" s="302"/>
       <c r="S5" s="205" t="s">
         <v>111</v>
       </c>
@@ -7736,11 +7744,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -7757,6 +7760,11 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7768,8 +7776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI252"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -19300,7 +19308,7 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -25010,4 +25018,410 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.94488188976377963" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C4:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:6">
+      <c r="C4" s="154"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="158"/>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="C5" s="154" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="152"/>
+      <c r="E5" s="151">
+        <v>50888</v>
+      </c>
+      <c r="F5" s="158" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6" s="154" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="105"/>
+      <c r="E6" s="151">
+        <v>30848</v>
+      </c>
+      <c r="F6" s="152" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="C7" s="154" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="152"/>
+      <c r="E7" s="151">
+        <v>43910</v>
+      </c>
+      <c r="F7" s="158" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="C8" s="154" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="105"/>
+      <c r="E8" s="151">
+        <v>25872</v>
+      </c>
+      <c r="F8" s="158" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="C9" s="150" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="105"/>
+      <c r="E9" s="151">
+        <v>9570</v>
+      </c>
+      <c r="F9" s="158" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10" s="150" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="105"/>
+      <c r="E10" s="151">
+        <v>40540</v>
+      </c>
+      <c r="F10" s="158" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11" s="154" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="105"/>
+      <c r="E11" s="151">
+        <v>23800</v>
+      </c>
+      <c r="F11" s="152" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6">
+      <c r="C12" s="154" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="105"/>
+      <c r="E12" s="151">
+        <v>25276</v>
+      </c>
+      <c r="F12" s="155" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6">
+      <c r="C13" s="154" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="152"/>
+      <c r="E13" s="151">
+        <v>2400</v>
+      </c>
+      <c r="F13" s="152" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="C14" s="154" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="105"/>
+      <c r="E14" s="151">
+        <v>44000</v>
+      </c>
+      <c r="F14" s="158" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6">
+      <c r="C15" s="154"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="155"/>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="C16" s="150"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="155"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="154"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="158"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="154"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="155"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="154"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="155"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="154"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="155"/>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="154"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="151"/>
+      <c r="F21" s="155"/>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="154"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="246"/>
+      <c r="F22" s="155"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="150"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="151"/>
+      <c r="F23" s="158"/>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="154"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="151"/>
+      <c r="F24" s="155"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="154"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="158"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="154"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="151"/>
+      <c r="F26" s="152"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="154"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="155"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="154"/>
+      <c r="D28" s="105"/>
+      <c r="E28" s="151"/>
+      <c r="F28" s="155"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="150"/>
+      <c r="D29" s="158"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="155"/>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="150"/>
+      <c r="D30" s="105"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="155"/>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="154"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="151"/>
+      <c r="F31" s="155"/>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="154"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="152"/>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="154"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="151"/>
+      <c r="F33" s="155"/>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="154"/>
+      <c r="D34" s="105"/>
+      <c r="E34" s="151"/>
+      <c r="F34" s="152"/>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" s="154"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="151"/>
+      <c r="F35" s="152"/>
+    </row>
+  </sheetData>
+  <sortState ref="C5:F35">
+    <sortCondition ref="C5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="154" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="151">
+        <v>50888</v>
+      </c>
+      <c r="C1" s="151" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="154" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="151">
+        <v>30848</v>
+      </c>
+      <c r="C2" s="329" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="154" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="151">
+        <v>43910</v>
+      </c>
+      <c r="C3" s="151" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="154" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="151">
+        <v>25872</v>
+      </c>
+      <c r="C4" s="151" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="150" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="151">
+        <v>9570</v>
+      </c>
+      <c r="C5" s="151" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="150" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="151">
+        <v>40540</v>
+      </c>
+      <c r="C6" s="151" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="154" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="151">
+        <v>23800</v>
+      </c>
+      <c r="C7" s="329" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="154" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="151">
+        <v>25276</v>
+      </c>
+      <c r="C8" s="330" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="154" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="151">
+        <v>2400</v>
+      </c>
+      <c r="C9" s="329" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="154" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="151">
+        <v>44000</v>
+      </c>
+      <c r="C10" s="151" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="300" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>